<commit_message>
dmz reverse proxy; TOGAF docs
</commit_message>
<xml_diff>
--- a/docs/McSOC IPPLAN.xlsx
+++ b/docs/McSOC IPPLAN.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="90">
   <si>
     <t>host</t>
   </si>
@@ -30,6 +30,9 @@
     <t>ipaddr</t>
   </si>
   <si>
+    <t>ssh port</t>
+  </si>
+  <si>
     <t>connection</t>
   </si>
   <si>
@@ -141,6 +144,27 @@
     <t>10.10.11.1</t>
   </si>
   <si>
+    <t>dmzdns</t>
+  </si>
+  <si>
+    <t>dmzmail</t>
+  </si>
+  <si>
+    <t>10.10.3.3</t>
+  </si>
+  <si>
+    <t>dmzweb</t>
+  </si>
+  <si>
+    <t>10.10.3.4</t>
+  </si>
+  <si>
+    <t>proxy</t>
+  </si>
+  <si>
+    <t>10.10.3.5</t>
+  </si>
+  <si>
     <t>nagios</t>
   </si>
   <si>
@@ -160,6 +184,24 @@
   </si>
   <si>
     <t>10.10.8.11</t>
+  </si>
+  <si>
+    <t>mail</t>
+  </si>
+  <si>
+    <t>10.10.8.13</t>
+  </si>
+  <si>
+    <t>web</t>
+  </si>
+  <si>
+    <t>10.10.8.14</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>10.10.8.15</t>
   </si>
   <si>
     <t>entwks101</t>
@@ -424,18 +466,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.280612244898"/>
     <col collapsed="false" hidden="false" max="4" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6377551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -454,400 +497,647 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>22101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>22102</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>22103</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>22104</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>22105</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>42</v>
+        <v>9</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>22301</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>22302</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>22304</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>22303</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="0" t="s">
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>49</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>22401</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>22402</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>22801</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>22903</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>22904</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>22905</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>22901</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -885,27 +1175,27 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>443</v>
@@ -914,18 +1204,18 @@
         <v>55433</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>443</v>
@@ -934,18 +1224,18 @@
         <v>55434</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>443</v>
@@ -954,18 +1244,18 @@
         <v>55435</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>443</v>
@@ -974,18 +1264,18 @@
         <v>55436</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>443</v>
@@ -994,18 +1284,18 @@
         <v>55437</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>80</v>
@@ -1014,309 +1304,309 @@
         <v>18033</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>80</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>631</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>12320</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>12321</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>139</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>445</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>22</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>443</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>631</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>6556</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>80</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>135</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>3268</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>3269</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>1024</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>464</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>53</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>636</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>88</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>